<commit_message>
[master] finished laravel assignment_02
</commit_message>
<xml_diff>
--- a/laravels/Laravel_review_points_WaiLinOo.xlsx
+++ b/laravels/Laravel_review_points_WaiLinOo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>№</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>WaiLinOo</t>
+  </si>
+  <si>
+    <t>Export and import file</t>
+  </si>
+  <si>
+    <t>1)url tway route name tway ko (e.g. export-excel) 2)function name tway lowerCamelCase 3)request validataion 4)custom error message</t>
   </si>
   <si>
     <t>エラータイプ</t>
@@ -120,8 +126,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -138,7 +144,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,32 +172,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,6 +203,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -228,16 +226,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -252,14 +257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,6 +273,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -282,13 +288,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,31 +321,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,151 +483,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,21 +629,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -705,6 +678,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -729,162 +726,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1891,11 +1879,11 @@
   <sheetPr/>
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="5.44166666666667" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.1083333333333" style="3" customWidth="1"/>
@@ -2011,29 +1999,51 @@
       <c r="X2" s="29"/>
     </row>
     <row r="3" ht="123" customHeight="1" spans="1:24">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>44566</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="17"/>
+      <c r="I3" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="23"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="24"/>
+      <c r="O3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
       <c r="S3" s="30"/>
       <c r="T3" s="30"/>
       <c r="U3" s="31"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
+      <c r="V3" s="28">
+        <v>44566</v>
+      </c>
+      <c r="W3" s="29" t="s">
+        <v>19</v>
+      </c>
       <c r="X3" s="29"/>
     </row>
     <row r="4" ht="214.5" customHeight="1" spans="1:24">
@@ -2329,7 +2339,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2343,10 +2353,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -2357,10 +2367,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -2370,13 +2380,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2385,7 +2395,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2394,7 +2404,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2403,7 +2413,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
[master] finished laravel assignment_03 and review update
</commit_message>
<xml_diff>
--- a/laravels/Laravel_review_points_WaiLinOo.xlsx
+++ b/laravels/Laravel_review_points_WaiLinOo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>№</t>
   </si>
@@ -86,7 +86,12 @@
     <t>Export and import file</t>
   </si>
   <si>
-    <t>1)url tway route name tway ko (e.g. export-excel) 2)function name tway lowerCamelCase 3)request validataion 4)custom error message</t>
+    <t>1) Use Form Request validation and custom messages
+2) Keep old value of already filled fields when validate ( for create &amp; edit form page )
+3) Please use soft delete in delete process to remain deleted data in db</t>
+  </si>
+  <si>
+    <t>complete(soft delete remain)</t>
   </si>
   <si>
     <t>エラータイプ</t>
@@ -124,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -144,6 +149,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -153,12 +165,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -181,7 +194,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,14 +216,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -226,11 +231,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -242,15 +254,31 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,30 +293,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,6 +326,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -333,157 +464,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,6 +634,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -668,11 +682,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,21 +721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -731,15 +736,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -749,130 +754,130 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1879,8 +1884,8 @@
   <sheetPr/>
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:U4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2031,7 +2036,7 @@
         <v>17</v>
       </c>
       <c r="P3" s="24" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
@@ -2339,7 +2344,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2353,10 +2358,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -2367,10 +2372,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -2380,13 +2385,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2395,7 +2400,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2404,7 +2409,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2413,7 +2418,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
[master] finished laravel assignment_05 mail and review update
</commit_message>
<xml_diff>
--- a/laravels/Laravel_review_points_WaiLinOo.xlsx
+++ b/laravels/Laravel_review_points_WaiLinOo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>№</t>
   </si>
@@ -83,7 +83,10 @@
     <t>WaiLinOo</t>
   </si>
   <si>
-    <t>Export and import file</t>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>assignment_01</t>
   </si>
   <si>
     <t>1) Use Form Request validation and custom messages
@@ -91,7 +94,27 @@
 3) Please use soft delete in delete process to remain deleted data in db</t>
   </si>
   <si>
-    <t>complete(soft delete remain)</t>
+    <t>1) Delete confirmation in delete process.</t>
+  </si>
+  <si>
+    <t>assignment_02</t>
+  </si>
+  <si>
+    <t>1) Export PDF , no mojar name data 
+2) Export Excel , instead of major_id , export with major_name
+3) Export Csv , instead of major_id , export with major_name</t>
+  </si>
+  <si>
+    <t>assignment_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) After create process , click save , page is covered by modal </t>
+  </si>
+  <si>
+    <t>1) After update again and again , major name data are duplicated again and again.</t>
+  </si>
+  <si>
+    <t>1) When edit , major name data should be selected (data of student's major name from db).</t>
   </si>
   <si>
     <t>エラータイプ</t>
@@ -113,9 +136,6 @@
   </si>
   <si>
     <t>Leakage</t>
-  </si>
-  <si>
-    <t>Improvement</t>
   </si>
   <si>
     <t>Expression</t>
@@ -129,17 +149,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Meiryo"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -155,10 +181,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -169,17 +204,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,7 +228,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,7 +243,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -239,10 +273,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,23 +289,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,15 +311,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,12 +346,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -338,13 +484,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,139 +532,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,9 +680,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,15 +728,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -678,6 +739,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -697,21 +767,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -720,168 +775,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -922,6 +966,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -933,9 +989,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -947,12 +1000,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1184,6 +1231,125 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>50799</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1102363</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1117599</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1626729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6002020" y="5872480"/>
+          <a:ext cx="4495800" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>42334</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>220135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1134534</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2376822</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5993765" y="6788150"/>
+          <a:ext cx="4521200" cy="2157095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>296333</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>868648</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2472267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6933565" y="9321800"/>
+          <a:ext cx="3315335" cy="2294255"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1456,420 +1622,420 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="38"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="39"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="39"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="39"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="39"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="39"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="39"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="40"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="39"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="39"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="40"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="39"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="40"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="39"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="40"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="39"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="40"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="39"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="40"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="39"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="40"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="34"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="39"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="40"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="39"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="40"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="39"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="40"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="39"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="40"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="39"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="40"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="39"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="40"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="39"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="40"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="39"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="40"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="34"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="39"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="40"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="39"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="40"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="39"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="40"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="39"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="40"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="40"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1884,8 +2050,8 @@
   <sheetPr/>
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:U3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1894,7 +2060,7 @@
     <col min="2" max="2" width="13.1083333333333" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.3333333333333" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.66666666666667" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.4416666666667" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5583333333333" style="3" customWidth="1"/>
     <col min="6" max="13" width="9" style="3"/>
     <col min="14" max="14" width="17.6666666666667" style="3" customWidth="1"/>
     <col min="15" max="15" width="13" style="3" customWidth="1"/>
@@ -1937,21 +2103,21 @@
       <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="27" t="s">
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1976,32 +2142,32 @@
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="20" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="28">
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="29">
         <v>44564</v>
       </c>
-      <c r="W2" s="29" t="s">
+      <c r="W2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="29"/>
+      <c r="X2" s="30"/>
     </row>
     <row r="3" ht="123" customHeight="1" spans="1:24">
       <c r="A3" s="9">
@@ -2017,169 +2183,261 @@
         <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="29">
+        <v>44566</v>
+      </c>
+      <c r="W3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" s="30"/>
+    </row>
+    <row r="4" ht="54" customHeight="1" spans="1:24">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>44571</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="20" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="28">
-        <v>44566</v>
-      </c>
-      <c r="W3" s="29" t="s">
+      <c r="P4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="29">
+        <v>44571</v>
+      </c>
+      <c r="W4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="29"/>
-    </row>
-    <row r="4" ht="214.5" customHeight="1" spans="1:24">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-    </row>
-    <row r="5" ht="214.5" customHeight="1" spans="1:24">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-    </row>
-    <row r="6" ht="246.75" customHeight="1" spans="1:24">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-    </row>
-    <row r="7" ht="285" customHeight="1" spans="1:24">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-    </row>
-    <row r="8" ht="106.5" customHeight="1" spans="1:24">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
+      <c r="X4" s="30"/>
+    </row>
+    <row r="5" ht="141.6" customHeight="1" spans="1:24">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>44571</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="29">
+        <v>44571</v>
+      </c>
+      <c r="W5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="X5" s="30"/>
+    </row>
+    <row r="6" ht="202.8" customHeight="1" spans="1:24">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>44571</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+    </row>
+    <row r="7" ht="197.4" customHeight="1" spans="1:24">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>44571</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+    </row>
+    <row r="8" ht="51.6" customHeight="1" spans="1:24">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>44571</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="30"/>
     </row>
     <row r="9" ht="106.5" customHeight="1" spans="1:24">
       <c r="A9" s="9"/>
@@ -2187,25 +2445,25 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
     </row>
     <row r="10" ht="106.5" customHeight="1" spans="1:24">
       <c r="A10" s="9"/>
@@ -2213,25 +2471,25 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
     </row>
     <row r="11" ht="139.5" customHeight="1" spans="1:24">
       <c r="A11" s="9"/>
@@ -2239,25 +2497,25 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -2315,6 +2573,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2344,7 +2603,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2358,10 +2617,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -2372,10 +2631,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -2385,13 +2644,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2400,7 +2659,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2409,7 +2668,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2418,7 +2677,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
[master] finished laravel tutorial_05 and review update fianl
</commit_message>
<xml_diff>
--- a/laravels/Laravel_review_points_WaiLinOo.xlsx
+++ b/laravels/Laravel_review_points_WaiLinOo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>№</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>1) When edit , major name data should be selected (data of student's major name from db).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assignment_05 and all </t>
+  </si>
+  <si>
+    <t>1)use laravel with() 2)write function doc 3)write db code in DAO 4)use form request 5)use DB transaction 6)add else condition</t>
   </si>
   <si>
     <t>エラータイプ</t>
@@ -151,8 +157,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -168,24 +174,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,6 +196,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -207,7 +226,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,20 +287,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,13 +324,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -346,13 +352,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +460,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,43 +496,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,97 +520,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,6 +666,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -684,50 +729,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,148 +768,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2030,7 +2036,7 @@
   <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2437,29 +2443,51 @@
       <c r="X8" s="29"/>
     </row>
     <row r="9" ht="106.5" customHeight="1" spans="1:24">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>44572</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="16"/>
+      <c r="I9" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
       <c r="N9" s="18"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="24"/>
+      <c r="O9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="Q9" s="30"/>
       <c r="R9" s="30"/>
       <c r="S9" s="30"/>
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
+      <c r="V9" s="28">
+        <v>44572</v>
+      </c>
+      <c r="W9" s="29" t="s">
+        <v>19</v>
+      </c>
       <c r="X9" s="29"/>
     </row>
     <row r="10" ht="106.5" customHeight="1" spans="1:24">
@@ -2600,7 +2628,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2614,10 +2642,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -2628,10 +2656,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -2641,13 +2669,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2665,7 +2693,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2674,7 +2702,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>